<commit_message>
updated files in config dir; Simon
</commit_message>
<xml_diff>
--- a/config/important_protein_names.xlsx
+++ b/config/important_protein_names.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
   <si>
-    <t xml:space="preserve">&gt; Signaling of Hepatocyte Growth Factor Receptor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; TGF-beta signaling pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; EGF Signaling Pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; EPO Signaling Pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; GAS6 Signaling Pathway</t>
+    <t xml:space="preserve">Signaling of Hepatocyte Growth Factor Receptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGF-beta signaling pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGF Signaling Pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPO Signaling Pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAS6 Signaling Pathway</t>
   </si>
   <si>
     <t xml:space="preserve">ACTA1</t>
@@ -673,7 +673,7 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,7 +684,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.79"/>
   </cols>
   <sheetData>

</xml_diff>